<commit_message>
debug check for full rows of missing data
</commit_message>
<xml_diff>
--- a/product_data/processing_metadata/C5/PROF_meta.xlsx
+++ b/product_data/processing_metadata/C5/PROF_meta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitytasmania-my.sharepoint.com/personal/kimberlee_baldry_utas_edu_au/Documents/Documents/Projects/BIO-MATE/BIO-MATE/product_data/processing_metadata/C5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="235" documentId="13_ncr:1_{8B370A32-E872-4C94-946E-4B177D89299C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FA21212-156A-45B2-A631-ACDBF310AD44}"/>
+  <xr:revisionPtr revIDLastSave="256" documentId="13_ncr:1_{8B370A32-E872-4C94-946E-4B177D89299C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD52E7F7-C03F-4601-BB49-AD71F1ADBAD3}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E6D5457A-6BC7-4401-B590-10CB8DC6A801}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6D5457A-6BC7-4401-B590-10CB8DC6A801}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="193">
   <si>
     <t>49NZ20031209</t>
   </si>
@@ -435,18 +435,9 @@
     <t>gregory.c.johnson@noaa.gov</t>
   </si>
   <si>
-    <t>E:/Data_downloads/PANGEAE/91AH20140402/chl</t>
-  </si>
-  <si>
-    <t>.tab</t>
-  </si>
-  <si>
     <t>PANGEA</t>
   </si>
   <si>
-    <t>tab</t>
-  </si>
-  <si>
     <t>Stephanie de Villiers</t>
   </si>
   <si>
@@ -465,9 +456,6 @@
     <t>Event</t>
   </si>
   <si>
-    <t>Date/Time</t>
-  </si>
-  <si>
     <t>%Y-%m-%dT%H:%M</t>
   </si>
   <si>
@@ -477,9 +465,6 @@
     <t>Longitude</t>
   </si>
   <si>
-    <t>Pres</t>
-  </si>
-  <si>
     <t>Temp</t>
   </si>
   <si>
@@ -516,12 +501,6 @@
     <t>Date.Time</t>
   </si>
   <si>
-    <t>%Y-%m-%dT%H:%M:S</t>
-  </si>
-  <si>
-    <t>Press..dbar.</t>
-  </si>
-  <si>
     <t>Chla</t>
   </si>
   <si>
@@ -625,6 +604,15 @@
   </si>
   <si>
     <t>garcial@etseccpb.upc.es</t>
+  </si>
+  <si>
+    <t>Press</t>
+  </si>
+  <si>
+    <t>E:/Data_downloads/TARA_PANGEAE/35XI20090905/ctd/split</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -1016,10 +1004,13 @@
   <dimension ref="A1:BA22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="5" max="5" width="13.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:53">
       <c r="A1" t="s">
@@ -2737,85 +2728,85 @@
         <v>65</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D12" t="s">
         <v>133</v>
-      </c>
-      <c r="D12" t="s">
-        <v>135</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F12" t="s">
+        <v>138</v>
+      </c>
+      <c r="G12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" t="s">
+        <v>134</v>
+      </c>
+      <c r="I12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="K12" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>139</v>
+      </c>
+      <c r="S12" t="s">
+        <v>154</v>
+      </c>
+      <c r="T12" t="s">
+        <v>140</v>
+      </c>
+      <c r="U12" t="s">
+        <v>154</v>
+      </c>
+      <c r="X12" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z12" t="s">
         <v>141</v>
       </c>
-      <c r="G12" t="s">
-        <v>136</v>
-      </c>
-      <c r="H12" t="s">
-        <v>137</v>
-      </c>
-      <c r="I12" t="s">
-        <v>138</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="K12" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q12" t="s">
+      <c r="AA12" t="s">
         <v>142</v>
-      </c>
-      <c r="S12" t="s">
-        <v>143</v>
-      </c>
-      <c r="T12" t="s">
-        <v>144</v>
-      </c>
-      <c r="U12" t="s">
-        <v>143</v>
-      </c>
-      <c r="X12" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>146</v>
       </c>
       <c r="AF12" t="s">
         <v>84</v>
       </c>
       <c r="AG12" t="s">
-        <v>147</v>
+        <v>190</v>
       </c>
       <c r="AH12" t="s">
         <v>85</v>
       </c>
       <c r="AI12" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="AJ12" t="s">
         <v>86</v>
       </c>
       <c r="AK12" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="AL12" t="s">
         <v>87</v>
       </c>
       <c r="AM12" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="AN12" t="s">
         <v>88</v>
       </c>
       <c r="AO12" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:53">
@@ -2826,79 +2817,82 @@
         <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>152</v>
+        <v>191</v>
       </c>
       <c r="D13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G13" t="s">
         <v>70</v>
       </c>
       <c r="H13" t="s">
+        <v>148</v>
+      </c>
+      <c r="I13" t="s">
+        <v>149</v>
+      </c>
+      <c r="J13" t="s">
+        <v>151</v>
+      </c>
+      <c r="K13" t="s">
+        <v>152</v>
+      </c>
+      <c r="N13" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q13" t="s">
         <v>153</v>
       </c>
-      <c r="I13" t="s">
+      <c r="S13" t="s">
         <v>154</v>
       </c>
-      <c r="J13" t="s">
-        <v>156</v>
-      </c>
-      <c r="K13" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>158</v>
-      </c>
-      <c r="S13" t="s">
-        <v>159</v>
-      </c>
       <c r="T13" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
       <c r="U13" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="X13" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
       <c r="Z13" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="AA13" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="AF13" t="s">
         <v>84</v>
       </c>
       <c r="AG13" t="s">
-        <v>161</v>
+        <v>190</v>
       </c>
       <c r="AH13" t="s">
         <v>85</v>
       </c>
       <c r="AI13" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="AJ13" t="s">
         <v>86</v>
       </c>
       <c r="AK13" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="AL13" t="s">
         <v>87</v>
       </c>
       <c r="AO13" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="AQ13" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="AR13" t="s">
         <v>96</v>
@@ -3067,7 +3061,7 @@
         <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D15" t="s">
         <v>68</v>
@@ -3076,22 +3070,22 @@
         <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="G15" t="s">
         <v>70</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="K15" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="M15" t="s">
         <v>73</v>
@@ -3175,7 +3169,7 @@
         <v>96</v>
       </c>
       <c r="AS15" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="AT15" t="s">
         <v>96</v>
@@ -3329,28 +3323,28 @@
         <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="D17" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>125</v>
       </c>
       <c r="F17" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G17" t="s">
         <v>70</v>
       </c>
       <c r="H17" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="I17" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="N17" s="6">
         <v>-99999</v>
@@ -3359,49 +3353,49 @@
         <v>75</v>
       </c>
       <c r="Q17" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="S17" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="T17" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="U17" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="X17" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="Z17" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="AA17" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="AF17" t="s">
         <v>84</v>
       </c>
       <c r="AG17" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="AH17" t="s">
         <v>85</v>
       </c>
       <c r="AI17" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="AJ17" t="s">
         <v>86</v>
       </c>
       <c r="AK17" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="AL17" t="s">
         <v>87</v>
       </c>
       <c r="AM17" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="AN17" t="s">
         <v>88</v>
@@ -3415,28 +3409,28 @@
         <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D18" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>126</v>
       </c>
       <c r="F18" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G18" t="s">
         <v>70</v>
       </c>
       <c r="H18" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="I18" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="N18" s="6">
         <v>-99999</v>
@@ -3445,49 +3439,49 @@
         <v>75</v>
       </c>
       <c r="Q18" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="S18" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="T18" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="U18" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="X18" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="Z18" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="AA18" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="AF18" t="s">
         <v>84</v>
       </c>
       <c r="AG18" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="AH18" t="s">
         <v>85</v>
       </c>
       <c r="AI18" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="AJ18" t="s">
         <v>86</v>
       </c>
       <c r="AK18" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="AL18" t="s">
         <v>87</v>
       </c>
       <c r="AM18" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="AN18" t="s">
         <v>88</v>
@@ -3501,25 +3495,25 @@
         <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="D19" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E19" t="s">
         <v>128</v>
       </c>
       <c r="F19" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G19" t="s">
         <v>70</v>
       </c>
       <c r="H19" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="I19" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="N19" s="6">
         <v>-99999</v>
@@ -3528,43 +3522,43 @@
         <v>75</v>
       </c>
       <c r="Q19" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="S19" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="T19" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="U19" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="X19" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="Z19" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="AA19" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="AF19" t="s">
         <v>84</v>
       </c>
       <c r="AG19" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="AH19" t="s">
         <v>85</v>
       </c>
       <c r="AI19" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="AJ19" t="s">
         <v>86</v>
       </c>
       <c r="AK19" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="AL19" t="s">
         <v>87</v>
@@ -3578,28 +3572,28 @@
         <v>66</v>
       </c>
       <c r="C20" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="D20" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E20" t="s">
         <v>127</v>
       </c>
       <c r="F20" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G20" t="s">
         <v>70</v>
       </c>
       <c r="H20" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="I20" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="N20" s="6">
         <v>-99999</v>
@@ -3608,43 +3602,43 @@
         <v>75</v>
       </c>
       <c r="Q20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="S20" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="T20" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="U20" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="X20" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="Z20" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="AA20" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="AF20" t="s">
         <v>84</v>
       </c>
       <c r="AG20" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="AH20" t="s">
         <v>85</v>
       </c>
       <c r="AI20" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="AJ20" t="s">
         <v>86</v>
       </c>
       <c r="AK20" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="AL20" t="s">
         <v>87</v>
@@ -3661,73 +3655,73 @@
         <v>66</v>
       </c>
       <c r="C21" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>122</v>
       </c>
       <c r="F21" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="G21" t="s">
-        <v>136</v>
+        <v>70</v>
       </c>
       <c r="H21" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="O21" t="s">
         <v>75</v>
       </c>
       <c r="Q21" t="s">
+        <v>139</v>
+      </c>
+      <c r="S21" t="s">
+        <v>186</v>
+      </c>
+      <c r="T21" t="s">
+        <v>140</v>
+      </c>
+      <c r="U21" t="s">
+        <v>186</v>
+      </c>
+      <c r="X21" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>141</v>
+      </c>
+      <c r="AA21" t="s">
         <v>142</v>
-      </c>
-      <c r="S21" t="s">
-        <v>193</v>
-      </c>
-      <c r="T21" t="s">
-        <v>144</v>
-      </c>
-      <c r="U21" t="s">
-        <v>143</v>
-      </c>
-      <c r="X21" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z21" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA21" t="s">
-        <v>146</v>
       </c>
       <c r="AF21" t="s">
         <v>84</v>
       </c>
       <c r="AG21" t="s">
-        <v>147</v>
+        <v>190</v>
       </c>
       <c r="AH21" t="s">
         <v>85</v>
       </c>
       <c r="AI21" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="AJ21" t="s">
         <v>86</v>
       </c>
       <c r="AK21" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="AL21" t="s">
         <v>87</v>
       </c>
       <c r="AO21" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:41">
@@ -3738,73 +3732,73 @@
         <v>66</v>
       </c>
       <c r="C22" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D22" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>123</v>
       </c>
       <c r="F22" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="G22" t="s">
-        <v>136</v>
+        <v>70</v>
       </c>
       <c r="H22" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="O22" t="s">
         <v>75</v>
       </c>
       <c r="Q22" t="s">
+        <v>139</v>
+      </c>
+      <c r="S22" t="s">
+        <v>186</v>
+      </c>
+      <c r="T22" t="s">
+        <v>140</v>
+      </c>
+      <c r="U22" t="s">
+        <v>186</v>
+      </c>
+      <c r="X22" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>141</v>
+      </c>
+      <c r="AA22" t="s">
         <v>142</v>
-      </c>
-      <c r="S22" t="s">
-        <v>193</v>
-      </c>
-      <c r="T22" t="s">
-        <v>144</v>
-      </c>
-      <c r="U22" t="s">
-        <v>143</v>
-      </c>
-      <c r="X22" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA22" t="s">
-        <v>146</v>
       </c>
       <c r="AF22" t="s">
         <v>84</v>
       </c>
       <c r="AG22" t="s">
-        <v>147</v>
+        <v>190</v>
       </c>
       <c r="AH22" t="s">
         <v>85</v>
       </c>
       <c r="AI22" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="AJ22" t="s">
         <v>86</v>
       </c>
       <c r="AK22" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="AL22" t="s">
         <v>87</v>
       </c>
       <c r="AO22" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
long time no commit
</commit_message>
<xml_diff>
--- a/product_data/processing_metadata/C5/PROF_meta.xlsx
+++ b/product_data/processing_metadata/C5/PROF_meta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitytasmania-my.sharepoint.com/personal/kimberlee_baldry_utas_edu_au/Documents/Documents/Projects/BIO-MATE/BIO-MATE/product_data/processing_metadata/C5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{AFD6FFAF-44F9-4ECC-823B-3BD3D1ABBAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{690BD356-4B02-442C-9D4F-D6EB6E66302D}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{AFD6FFAF-44F9-4ECC-823B-3BD3D1ABBAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14E5FE35-6C99-49DA-B782-95807BE7964D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E6D5457A-6BC7-4401-B590-10CB8DC6A801}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6D5457A-6BC7-4401-B590-10CB8DC6A801}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="190">
   <si>
     <t>49NZ20031209</t>
   </si>
@@ -601,6 +601,9 @@
   </si>
   <si>
     <t>PANGEAE</t>
+  </si>
+  <si>
+    <t>cast</t>
   </si>
 </sst>
 </file>
@@ -983,7 +986,7 @@
   <dimension ref="A1:BB18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2772,6 +2775,9 @@
       <c r="L12" s="1" t="s">
         <v>179</v>
       </c>
+      <c r="P12" t="s">
+        <v>75</v>
+      </c>
       <c r="R12" t="s">
         <v>134</v>
       </c>
@@ -2864,8 +2870,14 @@
       <c r="O13" t="s">
         <v>167</v>
       </c>
+      <c r="P13" t="s">
+        <v>75</v>
+      </c>
       <c r="R13" t="s">
         <v>147</v>
+      </c>
+      <c r="S13" t="s">
+        <v>189</v>
       </c>
       <c r="T13" t="s">
         <v>148</v>

</xml_diff>